<commit_message>
cambiar nombre de las dimensiones
</commit_message>
<xml_diff>
--- a/utils/cleaners/Marco_consolidacion/Dimensión 5.xlsx
+++ b/utils/cleaners/Marco_consolidacion/Dimensión 5.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E192"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1246,7 +1246,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1262,7 +1262,7 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1271,12 +1271,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1287,7 +1287,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1296,12 +1296,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1312,7 +1312,7 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1362,7 +1362,7 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1387,7 +1387,7 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1396,12 +1396,12 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1412,16 +1412,16 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1437,11 +1437,11 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1462,7 +1462,7 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1512,7 +1512,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1562,7 +1562,7 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -1587,16 +1587,16 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1606,17 +1606,17 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1626,18 +1626,18 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1646,12 +1646,12 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1662,21 +1662,21 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1687,21 +1687,21 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1712,11 +1712,11 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1737,11 +1737,11 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1762,11 +1762,11 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1787,11 +1787,11 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1812,7 +1812,7 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1837,7 +1837,7 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -1862,7 +1862,7 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -1887,7 +1887,7 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -1901,7 +1901,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -1912,7 +1912,7 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -1926,7 +1926,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -1937,7 +1937,7 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -2012,7 +2012,7 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -2087,7 +2087,7 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2112,7 +2112,7 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -2126,7 +2126,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2137,7 +2137,7 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2162,16 +2162,16 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2181,22 +2181,22 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2206,13 +2206,13 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -2237,7 +2237,7 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -2251,7 +2251,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2262,7 +2262,7 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -2276,7 +2276,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2287,7 +2287,7 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -2312,7 +2312,7 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2337,7 +2337,7 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -2362,7 +2362,7 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2387,7 +2387,7 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -2412,7 +2412,7 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -2437,11 +2437,11 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2451,7 +2451,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -2462,11 +2462,11 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2476,7 +2476,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2487,7 +2487,7 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -2496,7 +2496,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2512,7 +2512,7 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2537,7 +2537,7 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -2562,11 +2562,11 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2587,11 +2587,11 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2612,11 +2612,11 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2637,11 +2637,11 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2662,7 +2662,7 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -2701,7 +2701,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -2712,7 +2712,7 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -2726,7 +2726,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -2737,7 +2737,7 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
@@ -2762,7 +2762,7 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -2801,7 +2801,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -2812,7 +2812,7 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -2826,7 +2826,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -2837,7 +2837,7 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -2862,7 +2862,7 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -2876,7 +2876,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -2887,7 +2887,7 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -2912,11 +2912,11 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2937,11 +2937,11 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2962,7 +2962,7 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
@@ -2996,12 +2996,12 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -3012,7 +3012,7 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3037,7 +3037,7 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -3062,7 +3062,7 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -3112,7 +3112,7 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -3137,7 +3137,7 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -3151,7 +3151,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -3162,16 +3162,16 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3181,22 +3181,22 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>1A</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3206,17 +3206,17 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2A</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3237,7 +3237,7 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -3262,7 +3262,7 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
@@ -3287,7 +3287,7 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -3312,7 +3312,7 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -3326,7 +3326,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -3337,16 +3337,16 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3356,22 +3356,22 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2B</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3381,13 +3381,13 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -3412,11 +3412,11 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -3437,7 +3437,7 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3456,17 +3456,17 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>1B</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -3476,7 +3476,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -3487,11 +3487,11 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -3512,16 +3512,16 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3531,22 +3531,22 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2B</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3556,13 +3556,13 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>2A</t>
+          <t>1A</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -3587,7 +3587,7 @@
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
@@ -3612,16 +3612,16 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2A</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3631,13 +3631,13 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2A</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -3662,7 +3662,7 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -3687,7 +3687,7 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
@@ -3712,7 +3712,7 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -3737,7 +3737,7 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
@@ -3762,7 +3762,7 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -3801,7 +3801,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -3812,7 +3812,7 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -3837,7 +3837,7 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -3862,7 +3862,7 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
@@ -3887,7 +3887,7 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
@@ -3912,7 +3912,7 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -3937,7 +3937,7 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
@@ -3962,7 +3962,7 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -3987,7 +3987,7 @@
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
@@ -4012,7 +4012,7 @@
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -4037,7 +4037,7 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4062,7 +4062,7 @@
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
@@ -4076,7 +4076,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -4087,7 +4087,7 @@
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
@@ -4112,7 +4112,7 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
@@ -4126,7 +4126,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
@@ -4137,7 +4137,7 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
@@ -4151,7 +4151,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
@@ -4162,7 +4162,7 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
@@ -4176,7 +4176,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -4187,7 +4187,7 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
@@ -4212,7 +4212,7 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
@@ -4226,7 +4226,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -4237,7 +4237,7 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
@@ -4262,7 +4262,7 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
@@ -4276,7 +4276,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -4287,7 +4287,7 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
@@ -4301,7 +4301,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -4312,7 +4312,7 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
@@ -4337,7 +4337,7 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
@@ -4362,7 +4362,7 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
@@ -4387,7 +4387,7 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
@@ -4412,7 +4412,7 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -4437,7 +4437,7 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -4451,7 +4451,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
@@ -4462,11 +4462,11 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -4476,7 +4476,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
@@ -4487,7 +4487,7 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
@@ -4501,7 +4501,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
@@ -4512,7 +4512,7 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -4526,7 +4526,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
@@ -4537,11 +4537,11 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -4551,7 +4551,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
@@ -4562,7 +4562,7 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -4587,7 +4587,7 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -4612,7 +4612,7 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -4626,7 +4626,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
@@ -4637,32 +4637,32 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -4676,7 +4676,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
@@ -4687,11 +4687,11 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -4712,32 +4712,32 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
@@ -4746,12 +4746,12 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
@@ -4762,11 +4762,11 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -4787,7 +4787,7 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
@@ -4801,7 +4801,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
@@ -4812,7 +4812,7 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
@@ -4821,7 +4821,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -4837,7 +4837,7 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
@@ -4851,7 +4851,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
@@ -4862,7 +4862,7 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
@@ -4887,7 +4887,7 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
@@ -4896,7 +4896,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -4912,7 +4912,7 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
@@ -4926,7 +4926,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -4937,7 +4937,7 @@
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
@@ -4962,7 +4962,7 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
@@ -4987,7 +4987,7 @@
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
@@ -5012,7 +5012,7 @@
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
@@ -5026,7 +5026,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
@@ -5037,21 +5037,21 @@
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
@@ -5062,16 +5062,16 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -5081,47 +5081,47 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>1A</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -5137,16 +5137,16 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -5156,22 +5156,22 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -5181,13 +5181,13 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>1B</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
@@ -5201,7 +5201,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
@@ -5212,24 +5212,99 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
+        <v>247</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>249</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>251</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
         <v>252</v>
       </c>
-      <c r="B192" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="C192" t="inlineStr">
-        <is>
-          <t>1A</t>
-        </is>
-      </c>
-      <c r="D192" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E192" t="inlineStr">
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
         <is>
           <t>1A</t>
         </is>

</xml_diff>